<commit_message>
modificaciones algoritmos recursivos – Laboratorio 5_Daniel
</commit_message>
<xml_diff>
--- a/Docs/Observaciones-lab4.xlsx
+++ b/Docs/Observaciones-lab4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisf\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/d_santos3_uniandes_edu_co/Documents/Séptimo semestre/Estructuras de datos y algoritmos/Reto1-G01/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF881AD3-E47C-44F9-838F-A66BD0DD5755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{AF881AD3-E47C-44F9-838F-A66BD0DD5755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E74DFFA8-C5C9-4CF1-914D-BE62328945B3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0CC1E4EA-1589-44BB-9685-B21706C2D41E}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{0CC1E4EA-1589-44BB-9685-B21706C2D41E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="70">
   <si>
     <t>Máquina 1</t>
   </si>
@@ -244,14 +244,28 @@
   </si>
   <si>
     <t>74022.33</t>
+  </si>
+  <si>
+    <t>Quick_sort</t>
+  </si>
+  <si>
+    <t>Merge_sort</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -294,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -314,6 +328,10 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -356,17 +374,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Reporte_Daniel!$I$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Insertion (Array_list)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -391,50 +398,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Reporte_Daniel!$H$4:$H$7</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Reporte_Daniel!$I$4:$I$7</c:f>
+              <c:f>Reporte_Daniel!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>36.97</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>588.84</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3899.79</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16203.72</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Reporte_Daniel!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>#REF!</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredCategoryTitle>
+                <c15:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Reporte_Daniel!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                  </c:numRef>
+                </c15:cat>
+              </c15:filteredCategoryTitle>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-93B5-44D1-9BC3-78B89ABCAFBF}"/>
             </c:ext>
@@ -443,17 +456,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Reporte_Daniel!$J$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Insertion ( Single_linked)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -478,50 +480,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Reporte_Daniel!$H$4:$H$7</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Reporte_Daniel!$J$4:$J$7</c:f>
+              <c:f>Reporte_Daniel!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>634</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41722.93</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>687799</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Reporte_Daniel!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>#REF!</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredCategoryTitle>
+                <c15:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Reporte_Daniel!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                  </c:numRef>
+                </c15:cat>
+              </c15:filteredCategoryTitle>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-93B5-44D1-9BC3-78B89ABCAFBF}"/>
             </c:ext>
@@ -657,6 +665,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10710127599111585"/>
+          <c:y val="0.88832719142430427"/>
+          <c:w val="0.85223734622307312"/>
+          <c:h val="7.5758105994326461E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -755,7 +773,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reporte_Daniel!$M$3</c:f>
+              <c:f>Reporte_Daniel!$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -778,7 +796,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Reporte_Daniel!$L$4:$L$7</c:f>
+              <c:f>Reporte_Daniel!$I$4:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -799,7 +817,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Reporte_Daniel!$M$4:$M$7</c:f>
+              <c:f>Reporte_Daniel!$J$4:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -830,7 +848,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reporte_Daniel!$N$3</c:f>
+              <c:f>Reporte_Daniel!$K$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -853,7 +871,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Reporte_Daniel!$L$4:$L$7</c:f>
+              <c:f>Reporte_Daniel!$I$4:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -874,7 +892,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Reporte_Daniel!$N$4:$N$7</c:f>
+              <c:f>Reporte_Daniel!$K$4:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1175,7 +1193,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reporte_Daniel!$Q$3</c:f>
+              <c:f>Reporte_Daniel!$N$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1198,7 +1216,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Reporte_Daniel!$P$4:$P$7</c:f>
+              <c:f>Reporte_Daniel!$M$4:$M$7</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1219,7 +1237,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Reporte_Daniel!$Q$4:$Q$7</c:f>
+              <c:f>Reporte_Daniel!$N$4:$N$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1250,7 +1268,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reporte_Daniel!$R$3</c:f>
+              <c:f>Reporte_Daniel!$O$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1273,7 +1291,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Reporte_Daniel!$P$4:$P$7</c:f>
+              <c:f>Reporte_Daniel!$M$4:$M$7</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1294,7 +1312,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Reporte_Daniel!$R$4:$R$7</c:f>
+              <c:f>Reporte_Daniel!$O$4:$O$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1570,6 +1588,642 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Reporte_Daniel!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2451</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4903</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Reporte_Daniel!$H$4:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.93</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>187.22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7A27-4F81-8152-F77BC0BDE58D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1025428703"/>
+        <c:axId val="1025429119"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1025428703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1025429119"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1025429119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1025428703"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Reporte_Daniel!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2451</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4903</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Reporte_Daniel!$G$4:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79.349999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>174.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BD43-4441-BDB4-DC20CCCF3D5D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1033436623"/>
+        <c:axId val="1033437039"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1033436623"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1033437039"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1033437039"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1033436623"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1690,6 +2344,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3238,20 +3972,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>594880</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>90054</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>642505</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>61479</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3278,15 +5044,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>885825</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>626052</xdr:colOff>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>623454</xdr:colOff>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3317,16 +5083,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1071995</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>93518</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>559377</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>150668</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3349,6 +5115,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>707046</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>13188</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>729027</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>89388</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C433623F-3A33-D833-50F4-77C8B8753B5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1322510</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>93785</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>40298</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>169985</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AAA75A3-A1B1-8DCF-659E-48FDDB65E53B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3656,7 +5494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32840A7A-E11C-45AB-AAB3-90B863B9180B}">
   <dimension ref="B2:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -3729,10 +5567,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DCD936-97B5-4C93-A9C5-4D6719EAA5B6}">
-  <dimension ref="B3:R20"/>
+  <dimension ref="B3:O20"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3:R7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3750,7 +5588,7 @@
     <col min="18" max="18" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
@@ -3766,30 +5604,28 @@
       <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="G3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="10"/>
       <c r="J3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="K3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="6"/>
       <c r="N3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>5</v>
       </c>
@@ -3805,36 +5641,33 @@
       <c r="F4" s="1">
         <v>33.659999999999997</v>
       </c>
-      <c r="H4" s="8">
+      <c r="G4" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="H4" s="2">
+        <f>4.93</f>
+        <v>4.93</v>
+      </c>
+      <c r="I4" s="8">
         <v>0.05</v>
       </c>
-      <c r="I4" s="2">
-        <v>36.97</v>
-      </c>
       <c r="J4" s="2">
-        <v>634</v>
-      </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="8">
+        <v>58.5</v>
+      </c>
+      <c r="K4" s="2">
+        <v>591.62</v>
+      </c>
+      <c r="M4" s="8">
         <v>0.05</v>
       </c>
-      <c r="M4" s="2">
-        <v>58.5</v>
-      </c>
       <c r="N4" s="2">
-        <v>591.62</v>
-      </c>
-      <c r="P4" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="Q4" s="2">
         <v>33.659999999999997</v>
       </c>
-      <c r="R4" s="2">
+      <c r="O4" s="2">
         <v>90.35</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>20</v>
       </c>
@@ -3850,36 +5683,32 @@
       <c r="F5" s="1">
         <v>191.06</v>
       </c>
-      <c r="H5" s="8">
+      <c r="G5" s="1">
+        <v>27.4</v>
+      </c>
+      <c r="H5" s="2">
+        <v>27.18</v>
+      </c>
+      <c r="I5" s="8">
         <v>0.2</v>
       </c>
-      <c r="I5" s="2">
-        <v>588.84</v>
-      </c>
       <c r="J5" s="2">
-        <v>41722.93</v>
-      </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="8">
+        <v>967.52</v>
+      </c>
+      <c r="K5" s="2">
+        <v>38218.620000000003</v>
+      </c>
+      <c r="M5" s="8">
         <v>0.2</v>
       </c>
-      <c r="M5" s="2">
-        <v>967.52</v>
-      </c>
       <c r="N5" s="2">
-        <v>38218.620000000003</v>
-      </c>
-      <c r="P5" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="Q5" s="2">
         <v>191.06</v>
       </c>
-      <c r="R5" s="2">
+      <c r="O5" s="2">
         <v>2255.34</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>50</v>
       </c>
@@ -3895,36 +5724,32 @@
       <c r="F6" s="1">
         <v>560.80999999999995</v>
       </c>
-      <c r="H6" s="8">
+      <c r="G6" s="1">
+        <v>79.349999999999994</v>
+      </c>
+      <c r="H6" s="2">
+        <v>88.8</v>
+      </c>
+      <c r="I6" s="8">
         <v>0.5</v>
       </c>
-      <c r="I6" s="2">
-        <v>3899.79</v>
-      </c>
       <c r="J6" s="2">
-        <v>687799</v>
-      </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="8">
+        <v>6167.97</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="8">
         <v>0.5</v>
       </c>
-      <c r="M6" s="2">
-        <v>6167.97</v>
-      </c>
       <c r="N6" s="2">
-        <v>0</v>
-      </c>
-      <c r="P6" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="Q6" s="2">
         <v>560.80999999999995</v>
       </c>
-      <c r="R6" s="2">
+      <c r="O6" s="2">
         <v>15928</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>100</v>
       </c>
@@ -3940,51 +5765,48 @@
       <c r="F7" s="1">
         <v>1436.84</v>
       </c>
-      <c r="H7" s="8">
+      <c r="G7" s="1">
+        <v>174.92</v>
+      </c>
+      <c r="H7" s="2">
+        <f>187.22</f>
+        <v>187.22</v>
+      </c>
+      <c r="I7" s="8">
         <v>1</v>
       </c>
-      <c r="I7" s="2">
-        <v>16203.72</v>
-      </c>
       <c r="J7" s="2">
+        <v>25672</v>
+      </c>
+      <c r="K7" s="2">
         <v>0</v>
       </c>
-      <c r="K7" s="6"/>
-      <c r="L7" s="8">
+      <c r="M7" s="8">
         <v>1</v>
       </c>
-      <c r="M7" s="2">
-        <v>25672</v>
-      </c>
       <c r="N7" s="2">
-        <v>0</v>
-      </c>
-      <c r="P7" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="2">
         <v>1436.84</v>
       </c>
-      <c r="R7" s="2">
+      <c r="O7" s="2">
         <v>82718.100000000006</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H12" s="7"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>